<commit_message>
Added workflow and normalized a videos
Former-commit-id: e298565bc94e5781c3876c34aa107bd6b7dcc56c
</commit_message>
<xml_diff>
--- a/3 Beginner Videos/Vid_3 Unclassified.xlsx
+++ b/3 Beginner Videos/Vid_3 Unclassified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/cjskalla_uiowa_edu/Documents/Documents/aerobictextreview/3 Beginner Videos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="952" documentId="11_F25DC773A252ABDACC1048EAE15952625BDE58EE" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2C0E1B45-FC90-4E33-80BA-333DF2B8A583}"/>
+  <xr:revisionPtr revIDLastSave="955" documentId="11_F25DC773A252ABDACC1048EAE15952625BDE58EE" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CC1C2083-8B53-4A6D-BDDE-F1BAB6122782}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="2835" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="445">
   <si>
     <t>vs</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>describing_body_understandable_to_novice</t>
-  </si>
-  <si>
-    <t>unclassified</t>
   </si>
   <si>
     <t>it's all standing</t>
@@ -246,9 +243,6 @@
     <t>nice deep breaths</t>
   </si>
   <si>
-    <t>engage work through</t>
-  </si>
-  <si>
     <t>you've got that water you've got that towel at any time you can go to it</t>
   </si>
   <si>
@@ -1382,6 +1376,9 @@
   </si>
   <si>
     <t>how'd it go for you Angie</t>
+  </si>
+  <si>
+    <t>engage, work through</t>
   </si>
 </sst>
 </file>
@@ -1705,11 +1702,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G269"/>
+  <dimension ref="A1:F270"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1720,10 +1717,9 @@
     <col min="4" max="4" width="9.140625" style="1"/>
     <col min="5" max="5" width="45.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1739,1981 +1735,1980 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="E13" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="1" t="s">
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="C18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E21" s="1" t="s">
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="C36" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="C49" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>325</v>
-      </c>
       <c r="E50" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="C61" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>383</v>
-      </c>
       <c r="E69" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E78" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E80" s="1" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E81" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E89" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E90" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E94" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E96" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E98" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+      <c r="E101" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E99" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E100" s="1" t="s">
+      <c r="E102" s="1" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E107" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+      <c r="E109" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E108" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+      <c r="E110" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E109" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+      <c r="E112" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E110" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+      <c r="E113" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E111" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="E114" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="E115" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+      <c r="E118" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E116" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="E119" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>156</v>
+        <v>228</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>231</v>
+        <v>154</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E136" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E137" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
+    <row r="142" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
         <v>256</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
         <v>280</v>
-      </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A161" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="167" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="179" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="181" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A181" s="1" t="s">
+    <row r="182" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
         <v>309</v>
-      </c>
-    </row>
-    <row r="182" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A182" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="1" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
         <v>314</v>
-      </c>
-    </row>
-    <row r="185" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A185" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A187" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="188" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="191" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="192" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="194" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A194" s="1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="195" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A195" s="1" t="s">
+    <row r="196" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="196" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A196" s="1" t="s">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
         <v>335</v>
-      </c>
-    </row>
-    <row r="197" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A197" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="199" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A199" s="1" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="200" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="201" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
         <v>341</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A203" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" s="1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="206" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
         <v>350</v>
-      </c>
-    </row>
-    <row r="209" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A209" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="210" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A210" s="1" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="211" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="215" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="216" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="219" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="220" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="224" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="225" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="232" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A232" s="1" t="s">
+    <row r="235" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
         <v>400</v>
-      </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="234" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A234" s="1" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A239" s="1" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="237" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A237" s="1" t="s">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="1" t="s">
         <v>408</v>
-      </c>
-    </row>
-    <row r="238" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A238" s="1" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" s="1" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="240" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A240" s="1" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="241" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="243" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="245" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="246" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="247" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="248" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
     </row>
     <row r="249" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="250" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A254" s="1" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="253" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A253" s="1" t="s">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A256" s="1" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" s="1" t="s">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="255" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A255" s="1" t="s">
+    <row r="258" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A258" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" s="1" t="s">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="1" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="257" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A257" s="1" t="s">
+    <row r="260" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" s="1" t="s">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="259" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A259" s="1" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" s="1" t="s">
+    <row r="262" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="261" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A261" s="1" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262" s="1" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="263" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="264" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="265" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A269" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
         <v>443</v>
-      </c>
-    </row>
-    <row r="268" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A268" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A269" s="1" t="s">
-        <v>445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>